<commit_message>
ISIS-1370: cleaning up the API to PublisherService, renaming EnlistedObjectsService to ChangedObjectsService etc.
</commit_message>
<xml_diff>
--- a/adocs/documentation/src/main/excel/command-dto-vs-interaction-dto-vs-interaction.xlsx
+++ b/adocs/documentation/src/main/excel/command-dto-vs-interaction-dto-vs-interaction.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
   <si>
     <t>InteractionDto</t>
   </si>
@@ -297,6 +297,54 @@
   </si>
   <si>
     <t>XMLGregorianCalendar completedAt</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>memberIdentifier</t>
+  </si>
+  <si>
+    <t>targetClass</t>
+  </si>
+  <si>
+    <t>targetAction</t>
+  </si>
+  <si>
+    <t>arguments</t>
+  </si>
+  <si>
+    <t>dto</t>
+  </si>
+  <si>
+    <t>memento</t>
+  </si>
+  <si>
+    <t>executeIn</t>
+  </si>
+  <si>
+    <t>startedAt</t>
+  </si>
+  <si>
+    <t>completedAt</t>
+  </si>
+  <si>
+    <t>exception</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>persistence</t>
+  </si>
+  <si>
+    <t>persistHint</t>
+  </si>
+  <si>
+    <t>timestamp</t>
   </si>
 </sst>
 </file>
@@ -360,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -396,6 +444,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,266 +746,341 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N33"/>
+  <dimension ref="A2:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" customWidth="1"/>
-    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46" style="6" customWidth="1"/>
-    <col min="6" max="6" width="35.5703125" customWidth="1"/>
-    <col min="7" max="7" width="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.85546875" customWidth="1"/>
-    <col min="9" max="9" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" customWidth="1"/>
+    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46" style="6" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" customWidth="1"/>
+    <col min="8" max="8" width="33" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.85546875" customWidth="1"/>
+    <col min="10" max="10" width="48.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" s="6" customFormat="1" ht="30">
+    <row r="2" spans="2:15" s="6" customFormat="1" ht="30">
       <c r="B2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="B4" s="2" t="s">
+    <row r="3" spans="2:15">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="2:15">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="2:15">
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="2:15">
+      <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
-      <c r="E7" s="9" t="s">
+    <row r="7" spans="2:15">
+      <c r="F7" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
-      <c r="E8" s="9" t="s">
+    <row r="8" spans="2:15">
+      <c r="F8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="B9" s="2" t="s">
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="2:15">
+      <c r="B9" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="1"/>
+      <c r="F9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="I9" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="E10" s="9"/>
-      <c r="G10" s="7" t="s">
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="2:15">
+      <c r="B10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="9"/>
+      <c r="I10" s="7"/>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="2:15">
+      <c r="F11" s="9"/>
+      <c r="H11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="G11" s="7" t="s">
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="2:15">
+      <c r="H12" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
-      <c r="B12" s="1"/>
-      <c r="D12" t="s">
+    <row r="13" spans="2:15">
+      <c r="C13" s="1"/>
+      <c r="E13" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="H13" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
-      <c r="C13" t="s">
+    <row r="14" spans="2:15">
+      <c r="D14" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F14" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="I14" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="B14" s="2" t="s">
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="2:15">
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="6" t="s">
+      <c r="E15" s="1"/>
+      <c r="F15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="I15" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="30">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="2:15">
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="1"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" ht="30">
+      <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" t="s">
+      <c r="B17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="F17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="I17" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="2" t="s">
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="2"/>
-      <c r="E16" s="9" t="s">
+      <c r="B18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="F18" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="I18" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="2" t="s">
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="B19" s="2"/>
+      <c r="D19" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="F19" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="I19" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
-      <c r="B18" s="2" t="s">
+    <row r="20" spans="1:10">
+      <c r="B20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="C20" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="E19" s="9" t="s">
+      <c r="F20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="F21" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="E20" s="9" t="s">
+    <row r="22" spans="1:10">
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I22" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
-      <c r="E21" s="9"/>
-      <c r="G21" s="7" t="s">
+    <row r="23" spans="1:10">
+      <c r="F23" s="9"/>
+      <c r="H23" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30">
-      <c r="E22" s="9" t="s">
+    <row r="24" spans="1:10" ht="30">
+      <c r="F24" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="H24" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="E23" s="9" t="s">
+    <row r="25" spans="1:10">
+      <c r="B25" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="9"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G26" t="s">
         <v>63</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="7" t="s">
+      <c r="H26" s="2"/>
+      <c r="I26" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
-      <c r="F24" t="s">
+    <row r="27" spans="1:10">
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" t="s">
         <v>64</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="7" t="s">
+      <c r="H27" s="2"/>
+      <c r="I27" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
-      <c r="H25" s="7" t="s">
+    <row r="28" spans="1:10">
+      <c r="I28" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
-      <c r="E27" s="10"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="E29" s="10"/>
-    </row>
-    <row r="33" spans="5:5">
-      <c r="E33"/>
+    <row r="29" spans="1:10">
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="10"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="B31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+      <c r="F32" s="10"/>
+    </row>
+    <row r="36" spans="6:6">
+      <c r="F36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>